<commit_message>
Login y Registrar usuario funcionales
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>Nombre Completo</t>
   </si>
@@ -29,16 +29,13 @@
     <t>Nivel</t>
   </si>
   <si>
-    <t>Juan</t>
+    <t>Id</t>
   </si>
   <si>
-    <t>JuanUsu</t>
+    <t>asd</t>
   </si>
   <si>
-    <t>Contra</t>
-  </si>
-  <si>
-    <t>correo@gmail</t>
+    <t>qwe</t>
   </si>
 </sst>
 </file>
@@ -83,7 +80,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
@@ -105,22 +102,48 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E2" t="n">
         <v>1.0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agrega el agregarfotos
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
   <si>
     <t>Nombre Completo</t>
   </si>
@@ -74,6 +74,18 @@
   </si>
   <si>
     <t>fff</t>
+  </si>
+  <si>
+    <t>SebastianJerez</t>
+  </si>
+  <si>
+    <t>Starjerez</t>
+  </si>
+  <si>
+    <t>27242679jsjs</t>
+  </si>
+  <si>
+    <t>sebastianjs99@hotmail.com</t>
   </si>
 </sst>
 </file>
@@ -426,7 +438,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
@@ -534,6 +546,26 @@
         <v>4.0</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Ascender usuario a colaborador y casi todos los botones del admin funcionales
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\univercidad\materias univercidad\semestre #3\Proyecto integrador\Motivator-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian\Documents\NetBeansProjects\Motivator-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2C6446-E1BA-49E4-8F63-A052CDEC977E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{022ECDE9-BC80-4D8F-849B-C32BEA6190D0}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="9420" windowWidth="17280" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="252"/>
   </bookViews>
   <sheets>
-    <sheet name="Usuarios" sheetId="1" r:id="rId1"/>
+    <sheet name="Usuarios" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
   <si>
     <t>Nombre Completo</t>
   </si>
@@ -101,6 +101,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -136,19 +137,19 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hipervínculo" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -165,10 +166,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -203,7 +204,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -255,7 +256,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -366,21 +367,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -397,7 +398,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -449,26 +450,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="28.21875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.44140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -524,8 +525,8 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E3">
-        <v>1</v>
+      <c r="E3" t="n">
+        <v>2.0</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -544,8 +545,8 @@
       <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="E4">
-        <v>1</v>
+      <c r="E4" t="n">
+        <v>3.0</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -584,8 +585,8 @@
       <c r="D6" t="s">
         <v>20</v>
       </c>
-      <c r="E6">
-        <v>1</v>
+      <c r="E6" t="n">
+        <v>3.0</v>
       </c>
       <c r="F6">
         <v>5</v>
@@ -613,8 +614,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D7" r:id="rId1" xr:uid="{BD998021-A1F0-47AC-A45E-CD5F43E249E7}"/>
+    <hyperlink r:id="rId1" ref="D7" xr:uid="{BD998021-A1F0-47AC-A45E-CD5F43E249E7}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ya no se cambian usuario y correo al ascender usuario
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian\Documents\NetBeansProjects\Motivator-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6DCA67-0B51-48B6-A748-513A01FB7E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A54E15C-DACD-4736-BF62-A20124D3D162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="2064" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="612" yWindow="3540" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Nombre Completo</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t>2724</t>
+  </si>
+  <si>
+    <t>zxc</t>
+  </si>
+  <si>
+    <t>@mail</t>
   </si>
 </sst>
 </file>
@@ -436,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -529,6 +535,26 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{D78EF421-0997-4E07-90E4-F7BC61A8385E}"/>

</xml_diff>

<commit_message>
Actualizacion de diseño del jFrame de ver lugares y actualizacion excel users
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\univercidad\materias univercidad\semestre #3\Proyecto integrador\Motivator-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C4F8C1-E264-45EC-9E2B-95D9DD9ECE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF161BF-C1B3-4457-94F0-91EFEC048892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,9 +82,6 @@
     <t>@mail</t>
   </si>
   <si>
-    <t>DavidGonzaloCordonFontecha</t>
-  </si>
-  <si>
     <t>Cordondavid532@gmail.com</t>
   </si>
   <si>
@@ -92,6 +89,9 @@
   </si>
   <si>
     <t>The_Cortux</t>
+  </si>
+  <si>
+    <t>David Gonzalo Cordon Fontecha</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,16 +569,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -591,8 +591,8 @@
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{D78EF421-0997-4E07-90E4-F7BC61A8385E}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{3A0596C1-82D5-4655-A8FE-51BBD6DFC374}"/>
-    <hyperlink ref="B6" r:id="rId3" display="Cordondavid532@gmail.com" xr:uid="{B2A97818-8514-40AA-B90F-2657E0099F6A}"/>
-    <hyperlink ref="D6" r:id="rId4" xr:uid="{A99D8190-0B52-40EC-AB2A-566ED497E03E}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{B2A97818-8514-40AA-B90F-2657E0099F6A}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{A99D8190-0B52-40EC-AB2A-566ED497E03E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
implementacion del boton desender
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\univercidad\materias univercidad\semestre #3\Proyecto integrador\Motivator-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF161BF-C1B3-4457-94F0-91EFEC048892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{6DF161BF-C1B3-4457-94F0-91EFEC048892}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="12456" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
   <sheets>
-    <sheet name="Usuarios" sheetId="1" r:id="rId1"/>
+    <sheet name="Usuarios" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
   <si>
     <t>Nombre Completo</t>
   </si>
@@ -98,6 +98,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -133,19 +134,19 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hipervínculo" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -162,10 +163,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -200,7 +201,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -252,7 +253,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -363,21 +364,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -394,7 +395,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -446,15 +447,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
@@ -462,9 +463,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.21875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.21875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -560,8 +561,8 @@
       <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="E5">
-        <v>1</v>
+      <c r="E5" t="n">
+        <v>1.0</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -589,12 +590,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{D78EF421-0997-4E07-90E4-F7BC61A8385E}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{3A0596C1-82D5-4655-A8FE-51BBD6DFC374}"/>
-    <hyperlink ref="D6" r:id="rId3" xr:uid="{B2A97818-8514-40AA-B90F-2657E0099F6A}"/>
-    <hyperlink ref="B6" r:id="rId4" xr:uid="{A99D8190-0B52-40EC-AB2A-566ED497E03E}"/>
+    <hyperlink r:id="rId1" ref="D2" xr:uid="{D78EF421-0997-4E07-90E4-F7BC61A8385E}"/>
+    <hyperlink r:id="rId2" ref="D3" xr:uid="{3A0596C1-82D5-4655-A8FE-51BBD6DFC374}"/>
+    <hyperlink r:id="rId3" ref="D6" xr:uid="{B2A97818-8514-40AA-B90F-2657E0099F6A}"/>
+    <hyperlink r:id="rId4" ref="B6" xr:uid="{A99D8190-0B52-40EC-AB2A-566ED497E03E}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Interfaz Ver Lugar e Inicio Usuario Actualizadas
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="24">
   <si>
     <t>Nombre Completo</t>
   </si>
@@ -581,8 +581,8 @@
       <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6">
-        <v>3</v>
+      <c r="E6" t="n">
+        <v>2.0</v>
       </c>
       <c r="F6">
         <v>5</v>

</xml_diff>

<commit_message>
TODAS LAS INTERFACES CON NUEVO DISENIO
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\univercidad\materias univercidad\semestre #3\Proyecto integrador\Motivator-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462606A5-61CA-4F3F-9ECE-2BBDB6381EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{6DF161BF-C1B3-4457-94F0-91EFEC048892}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="12456" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
   <sheets>
-    <sheet name="Usuarios" sheetId="1" r:id="rId1"/>
+    <sheet name="Usuarios" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="24">
   <si>
     <t>Nombre Completo</t>
   </si>
@@ -98,6 +98,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -133,19 +134,19 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hipervínculo" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -162,10 +163,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -200,7 +201,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -252,7 +253,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -363,21 +364,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -394,7 +395,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -446,25 +447,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.21875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.21875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -521,7 +522,7 @@
         <v>16</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -560,8 +561,8 @@
       <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="E5">
-        <v>1</v>
+      <c r="E5" t="n">
+        <v>1.0</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -580,8 +581,8 @@
       <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6">
-        <v>3</v>
+      <c r="E6" t="n">
+        <v>2.0</v>
       </c>
       <c r="F6">
         <v>5</v>
@@ -589,12 +590,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{D78EF421-0997-4E07-90E4-F7BC61A8385E}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{3A0596C1-82D5-4655-A8FE-51BBD6DFC374}"/>
-    <hyperlink ref="D6" r:id="rId3" xr:uid="{B2A97818-8514-40AA-B90F-2657E0099F6A}"/>
-    <hyperlink ref="B6" r:id="rId4" xr:uid="{A99D8190-0B52-40EC-AB2A-566ED497E03E}"/>
+    <hyperlink r:id="rId1" ref="D2" xr:uid="{D78EF421-0997-4E07-90E4-F7BC61A8385E}"/>
+    <hyperlink r:id="rId2" ref="D3" xr:uid="{3A0596C1-82D5-4655-A8FE-51BBD6DFC374}"/>
+    <hyperlink r:id="rId3" ref="D6" xr:uid="{B2A97818-8514-40AA-B90F-2657E0099F6A}"/>
+    <hyperlink r:id="rId4" ref="B6" xr:uid="{A99D8190-0B52-40EC-AB2A-566ED497E03E}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega codigo al nuevologin y nuevoregister
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\univercidad\materias univercidad\semestre #3\Proyecto integrador\Motivator-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documentos\NetBeansProjects\Motivator-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{6DF161BF-C1B3-4457-94F0-91EFEC048892}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C737AB-77A1-4BDE-9130-EC2EF6363D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="12456" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Usuarios" r:id="rId1" sheetId="1"/>
+    <sheet name="Usuarios" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Nombre Completo</t>
   </si>
@@ -40,65 +40,19 @@
     <t>Id</t>
   </si>
   <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>SebastianJerez</t>
-  </si>
-  <si>
-    <t>sebas</t>
-  </si>
-  <si>
-    <t>sebastianjs99@hotmail.com</t>
-  </si>
-  <si>
-    <t>qwe</t>
-  </si>
-  <si>
-    <t>JoseMartinez</t>
-  </si>
-  <si>
-    <t>Rex117</t>
-  </si>
-  <si>
-    <t>JulianGuardian</t>
-  </si>
-  <si>
-    <t>BloodSlayer</t>
-  </si>
-  <si>
-    <t>josemmp14@hotmail.com</t>
-  </si>
-  <si>
-    <t>andresvillamizar_g@hotmail.com</t>
-  </si>
-  <si>
-    <t>2724</t>
-  </si>
-  <si>
-    <t>zxc</t>
-  </si>
-  <si>
-    <t>@mail</t>
-  </si>
-  <si>
-    <t>Cordondavid532@gmail.com</t>
-  </si>
-  <si>
-    <t>Pinocho08</t>
-  </si>
-  <si>
-    <t>The_Cortux</t>
-  </si>
-  <si>
-    <t>David Gonzalo Cordon Fontecha</t>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>admin@admin.com</t>
+  </si>
+  <si>
+    <t>admin1234</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -134,19 +88,19 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hipervínculo" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -163,10 +117,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -201,7 +155,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -253,7 +207,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -364,21 +318,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -395,7 +349,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -447,28 +401,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.21875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.21875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="24.21875" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,114 +442,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E2">
         <v>3</v>
       </c>
       <c r="F2">
         <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="D2" xr:uid="{D78EF421-0997-4E07-90E4-F7BC61A8385E}"/>
-    <hyperlink r:id="rId2" ref="D3" xr:uid="{3A0596C1-82D5-4655-A8FE-51BBD6DFC374}"/>
-    <hyperlink r:id="rId3" ref="D6" xr:uid="{B2A97818-8514-40AA-B90F-2657E0099F6A}"/>
-    <hyperlink r:id="rId4" ref="B6" xr:uid="{A99D8190-0B52-40EC-AB2A-566ED497E03E}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{D78EF421-0997-4E07-90E4-F7BC61A8385E}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Parte de las interfaces de empresas listas (tienen errores de codigo debido a la falta de la clase empresa y sus metodos), interfaces que no se usaban eliminadas, algunos errores minimos corregidos
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documentos\NetBeansProjects\Motivator-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian\Documents\NetBeansProjects\Motivator-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1D3AF7-3D8A-4654-82AD-29F2535EBBEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374576ED-0F9C-4E9A-9767-A34958CEC737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4740" yWindow="2316" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Nombre Completo</t>
   </si>
@@ -71,6 +71,18 @@
   </si>
   <si>
     <t>pepito@pepito.com</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>jjuliang.2015@gmail.com</t>
+  </si>
+  <si>
+    <t>Julián Guardián</t>
+  </si>
+  <si>
+    <t>Blood</t>
   </si>
 </sst>
 </file>
@@ -422,20 +434,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,7 +467,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -475,7 +487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -495,7 +507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -513,6 +525,26 @@
       </c>
       <c r="F4">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Interfaz planes turisticos y empresas usuario, admin
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian\Documents\NetBeansProjects\Motivator-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374576ED-0F9C-4E9A-9767-A34958CEC737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{374576ED-0F9C-4E9A-9767-A34958CEC737}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="2316" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="9420" windowWidth="17280" xWindow="4740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="2316"/>
   </bookViews>
   <sheets>
-    <sheet name="Usuarios" sheetId="1" r:id="rId1"/>
+    <sheet name="Usuarios" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Nombre Completo</t>
   </si>
@@ -83,12 +83,22 @@
   </si>
   <si>
     <t>Blood</t>
+  </si>
+  <si>
+    <t>José</t>
+  </si>
+  <si>
+    <t>rex</t>
+  </si>
+  <si>
+    <t>cuentasfalsasxdd@hotmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -116,16 +126,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -142,10 +152,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -180,7 +190,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -232,7 +242,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -343,21 +353,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -374,7 +384,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -426,15 +436,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -442,9 +452,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.33203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -547,11 +557,31 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{D78EF421-0997-4E07-90E4-F7BC61A8385E}"/>
+    <hyperlink r:id="rId1" ref="D2" xr:uid="{D78EF421-0997-4E07-90E4-F7BC61A8385E}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>